<commit_message>
added static analog circuit test to report
</commit_message>
<xml_diff>
--- a/Lab9/Static Analog Circuit Test.xlsx
+++ b/Lab9/Static Analog Circuit Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel\Documents\EE445L\Lab9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEE611E-86B0-4327-AA56-CD0F4446599E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBED99E-C3DB-4F6F-A166-86611DD6947A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{3A54B06E-A497-4DDE-96C2-9AA9417B68FA}"/>
   </bookViews>
@@ -203,6 +203,106 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'static analog circuit test'!$B$1:$H$1</c:f>
@@ -1469,7 +1569,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>